<commit_message>
-Adjusted 3 notebooks for mode stats to get all values. plotted them. Also outputted sorted by total values into the excel.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_dichotomous_CRT.xlsx
+++ b/Data analytics/Language tests/Data/one_test_dichotomous_CRT.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olga\Documents\Projects\Data-Science-and-Machine-Learning\Data analytics\Language tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190B842F-E41F-48EA-8B86-175CADE2F99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AF9F0B-29F0-443D-AFF4-34F6DB17EC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="1035" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="4080" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:U31"/>
     </sheetView>
   </sheetViews>

</xml_diff>